<commit_message>
perbaikan struktur folder antara data raw dan data yang telah di preprocessing
</commit_message>
<xml_diff>
--- a/docs/korpus ABSA.xlsx
+++ b/docs/korpus ABSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\win 10\Documents\GitHub\ABSA-Transformer-Pemilu2024\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3D6247-223A-4E73-9FD5-688E91983FED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2381C37B-2E32-4CBF-86C1-74878D09D968}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{28524EF7-7997-43DF-AE7A-A35312A33E33}"/>
   </bookViews>
@@ -179,9 +179,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -189,6 +186,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE080EC-6008-4FCF-9C58-593DEE96D8FD}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -525,40 +525,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -593,74 +593,74 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -669,10 +669,10 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -681,22 +681,22 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="5"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -705,10 +705,10 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -717,10 +717,10 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -729,10 +729,10 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -741,10 +741,10 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -762,5 +762,6 @@
     <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>